<commit_message>
rerouting a little bit more
</commit_message>
<xml_diff>
--- a/Pieces.xlsx
+++ b/Pieces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\mini-rockets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83478C0-E332-4AD7-850B-B572BF1C8F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B4C208-F09D-4DFA-881E-FCC9CE60E688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7B2ECC38-15C7-4574-83EF-0C8BB6EF0B3C}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -888,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C5254F-CA5E-4BBF-8FA1-536629AE1229}">
   <dimension ref="G2:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
routage final completed avant review de plouffe
</commit_message>
<xml_diff>
--- a/Pieces.xlsx
+++ b/Pieces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\mini-rockets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B4C208-F09D-4DFA-881E-FCC9CE60E688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C3505B-DF2D-47DF-B8C8-3AAA6CBC8E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7B2ECC38-15C7-4574-83EF-0C8BB6EF0B3C}"/>
   </bookViews>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C5254F-CA5E-4BBF-8FA1-536629AE1229}">
   <dimension ref="G2:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
coder memory et main
</commit_message>
<xml_diff>
--- a/Pieces.xlsx
+++ b/Pieces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\mini-rockets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EF99F7-4EC2-4745-8A1D-474F9E486D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9035D12E-66DB-4759-AA67-19D2116F2C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7B2ECC38-15C7-4574-83EF-0C8BB6EF0B3C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7B2ECC38-15C7-4574-83EF-0C8BB6EF0B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="135">
   <si>
     <t>URL</t>
   </si>
@@ -314,15 +314,9 @@
     <t>SST25VF512A-33-4C-SAE</t>
   </si>
   <si>
-    <t>512 kb</t>
-  </si>
-  <si>
     <t>MS560702BA03-50</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/microchip-technology/SST25VF512A-33-4C-SAE/2297812</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/te-connectivity-measurement-specialties/MS560702BA03-50/4700931?s=N4IgTCBcDaILIGUCsA2ADAdjWAQgQTQGYBaJNEAXQF8g</t>
   </si>
   <si>
@@ -438,6 +432,15 @@
   </si>
   <si>
     <t>SST25VF016B-50-4C-S2AF-TCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/microchip-technology/SST25VF016B-50-4C-S2AF-T/2299430https://www.digikey.ca/en/products/detail/microchip-technology/SST25VF016B-50-4C-S2AF-T/2299430</t>
+  </si>
+  <si>
+    <t>16 mb</t>
+  </si>
+  <si>
+    <t>512 mb</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -650,7 +653,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -969,7 +971,7 @@
   <dimension ref="G2:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,17 +1008,17 @@
         <v>25</v>
       </c>
       <c r="I4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>20</v>
@@ -1214,7 +1216,7 @@
         <v>42</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="7:15" x14ac:dyDescent="0.25">
@@ -1259,10 +1261,10 @@
         <v>15</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="7:15" x14ac:dyDescent="0.25">
@@ -1283,10 +1285,10 @@
         <v>70</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="7:15" x14ac:dyDescent="0.25">
@@ -1334,7 +1336,7 @@
         <v>54</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="7:15" x14ac:dyDescent="0.25">
@@ -1390,7 +1392,7 @@
         <v>61</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I20" s="7">
         <v>100</v>
@@ -1429,10 +1431,10 @@
         <v>6</v>
       </c>
       <c r="N21" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="7:15" x14ac:dyDescent="0.25">
@@ -1477,10 +1479,10 @@
         <v>10</v>
       </c>
       <c r="N23" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="7:15" x14ac:dyDescent="0.25">
@@ -1501,7 +1503,7 @@
         <v>3</v>
       </c>
       <c r="N24" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O24" s="4" t="s">
         <v>75</v>
@@ -1525,10 +1527,10 @@
         <v>25</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="7:15" x14ac:dyDescent="0.25">
@@ -1584,7 +1586,7 @@
         <v>11</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="6">
@@ -1597,10 +1599,10 @@
         <v>3</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="7:15" x14ac:dyDescent="0.25">
@@ -1643,7 +1645,7 @@
         <v>3</v>
       </c>
       <c r="N30" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O30" s="4" t="s">
         <v>69</v>
@@ -1687,7 +1689,7 @@
         <v>9</v>
       </c>
       <c r="N32" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O32" s="4" t="s">
         <v>72</v>
@@ -1768,7 +1770,7 @@
         <v>5</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="I36" s="7">
         <v>7</v>
@@ -1777,16 +1779,16 @@
         <v>1</v>
       </c>
       <c r="L36">
-        <v>2.7</v>
+        <v>20</v>
       </c>
       <c r="M36" s="22">
         <v>3</v>
       </c>
-      <c r="N36" s="17" t="s">
-        <v>91</v>
+      <c r="N36" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="7:15" x14ac:dyDescent="0.25">
@@ -1807,10 +1809,10 @@
         <v>3</v>
       </c>
       <c r="N37" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="O37" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="O37" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="38" spans="7:15" x14ac:dyDescent="0.25">
@@ -1831,10 +1833,10 @@
         <v>3</v>
       </c>
       <c r="N38" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="7:15" x14ac:dyDescent="0.25">
@@ -1842,7 +1844,7 @@
         <v>18</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="6">
@@ -1855,15 +1857,15 @@
         <v>3</v>
       </c>
       <c r="N39" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="7:15" x14ac:dyDescent="0.25">
       <c r="G40" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H40" s="10"/>
       <c r="I40" s="10">
@@ -1880,10 +1882,10 @@
         <v>3</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O40" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="7:15" x14ac:dyDescent="0.25">
@@ -1897,19 +1899,25 @@
       </c>
       <c r="L41">
         <f t="shared" ref="L41" si="0">SUM(L5:L40)</f>
-        <v>340.44000000000005</v>
+        <v>357.74000000000007</v>
       </c>
       <c r="M41">
         <f>SUM(M5:M40)</f>
         <v>433</v>
       </c>
     </row>
-    <row r="44" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="L44">
-        <v>20</v>
-      </c>
-      <c r="N44" s="24" t="s">
-        <v>133</v>
+    <row r="43" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="L43">
+        <v>2.7</v>
+      </c>
+      <c r="N43" s="17" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="7:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1952,10 +1960,9 @@
     <hyperlink ref="O28" r:id="rId34" xr:uid="{1F63A02F-BC5D-4F6B-A97F-3AC85344D0B3}"/>
     <hyperlink ref="O40" r:id="rId35" xr:uid="{C400AB46-4FA9-4483-83AA-5FA6B84DA252}"/>
     <hyperlink ref="O13" r:id="rId36" xr:uid="{0078563A-E1CD-4AE8-B676-31D53AF7B7DA}"/>
-    <hyperlink ref="N44" r:id="rId37" display="https://www.digikey.ca/en/products/detail/microchip-technology/SST25VF016B-50-4C-S2AF-T/2299430" xr:uid="{775CBE35-EDAA-4D90-B75D-7ABB1CEC941E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -1963,7 +1970,7 @@
           <x14:formula1>
             <xm:f>Feuil2!$A$6:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>G47:G76 G21:G39 G5:G19</xm:sqref>
+          <xm:sqref>G47:G76 G21:G39 G5:G19 G43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{91638CD4-4D7E-4BF9-A735-AADB47737B6A}">
           <x14:formula1>
@@ -2085,7 +2092,7 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2109,35 +2116,35 @@
   <sheetData>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7">
         <v>512</v>
       </c>
       <c r="E7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D9">
         <v>3600000</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
@@ -2145,14 +2152,14 @@
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11">
         <f>D9/D6*D7</f>
         <v>92160000</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>